<commit_message>
scrapes entire district, clicks on next page
</commit_message>
<xml_diff>
--- a/storeData711.xlsx
+++ b/storeData711.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="73">
   <si>
     <t>county</t>
   </si>
@@ -161,6 +161,78 @@
   </si>
   <si>
     <t>基隆市中正區和一路125號127號</t>
+  </si>
+  <si>
+    <t>和豐</t>
+  </si>
+  <si>
+    <t>基隆市中正區新豐街203號1樓</t>
+  </si>
+  <si>
+    <t>哨船頭</t>
+  </si>
+  <si>
+    <t>基隆市中正區義一路43號1樓</t>
+  </si>
+  <si>
+    <t>海洋</t>
+  </si>
+  <si>
+    <t>基隆市中正區中正路609號1樓</t>
+  </si>
+  <si>
+    <t>財豐</t>
+  </si>
+  <si>
+    <t>基隆市中正區新豐街389號1樓</t>
+  </si>
+  <si>
+    <t>基義</t>
+  </si>
+  <si>
+    <t>基隆市中正區義二路181號185號1樓</t>
+  </si>
+  <si>
+    <t>港都</t>
+  </si>
+  <si>
+    <t>基隆市中正區義二路8號1樓</t>
+  </si>
+  <si>
+    <t>翔濱</t>
+  </si>
+  <si>
+    <t>基隆市中正區建國里祥豐街339號</t>
+  </si>
+  <si>
+    <t>新財發</t>
+  </si>
+  <si>
+    <t>基隆市中正區新豐街303巷11弄1號3號1樓</t>
+  </si>
+  <si>
+    <t>漁港</t>
+  </si>
+  <si>
+    <t>基隆市中正區中正路672號</t>
+  </si>
+  <si>
+    <t>龍騰</t>
+  </si>
+  <si>
+    <t>基隆市中正區義一路22號24號</t>
+  </si>
+  <si>
+    <t>豐勝</t>
+  </si>
+  <si>
+    <t>基隆市中正區中正路322號</t>
+  </si>
+  <si>
+    <t>觀山海</t>
+  </si>
+  <si>
+    <t>基隆市中正區砂子里觀海街49號51號1樓</t>
   </si>
 </sst>
 </file>
@@ -492,7 +564,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AM6"/>
+  <dimension ref="A1:AM18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -825,6 +897,474 @@
         <v>1</v>
       </c>
     </row>
+    <row r="7" spans="1:39">
+      <c r="C7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="Q7">
+        <v>1</v>
+      </c>
+      <c r="AB7">
+        <v>1</v>
+      </c>
+      <c r="AC7">
+        <v>1</v>
+      </c>
+      <c r="AI7">
+        <v>1</v>
+      </c>
+      <c r="AK7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:39">
+      <c r="C8" t="s">
+        <v>51</v>
+      </c>
+      <c r="D8" t="s">
+        <v>52</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="K8">
+        <v>1</v>
+      </c>
+      <c r="L8">
+        <v>1</v>
+      </c>
+      <c r="O8">
+        <v>1</v>
+      </c>
+      <c r="Q8">
+        <v>1</v>
+      </c>
+      <c r="R8">
+        <v>1</v>
+      </c>
+      <c r="T8">
+        <v>1</v>
+      </c>
+      <c r="AB8">
+        <v>1</v>
+      </c>
+      <c r="AC8">
+        <v>1</v>
+      </c>
+      <c r="AD8">
+        <v>1</v>
+      </c>
+      <c r="AI8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:39">
+      <c r="C9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D9" t="s">
+        <v>54</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="Q9">
+        <v>1</v>
+      </c>
+      <c r="R9">
+        <v>1</v>
+      </c>
+      <c r="S9">
+        <v>1</v>
+      </c>
+      <c r="T9">
+        <v>1</v>
+      </c>
+      <c r="U9">
+        <v>1</v>
+      </c>
+      <c r="Z9">
+        <v>1</v>
+      </c>
+      <c r="AB9">
+        <v>1</v>
+      </c>
+      <c r="AC9">
+        <v>1</v>
+      </c>
+      <c r="AD9">
+        <v>1</v>
+      </c>
+      <c r="AF9">
+        <v>1</v>
+      </c>
+      <c r="AH9">
+        <v>1</v>
+      </c>
+      <c r="AI9">
+        <v>1</v>
+      </c>
+      <c r="AJ9">
+        <v>1</v>
+      </c>
+      <c r="AK9">
+        <v>1</v>
+      </c>
+      <c r="AL9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:39">
+      <c r="C10" t="s">
+        <v>55</v>
+      </c>
+      <c r="D10" t="s">
+        <v>56</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="Q10">
+        <v>1</v>
+      </c>
+      <c r="R10">
+        <v>1</v>
+      </c>
+      <c r="S10">
+        <v>1</v>
+      </c>
+      <c r="AC10">
+        <v>1</v>
+      </c>
+      <c r="AD10">
+        <v>1</v>
+      </c>
+      <c r="AI10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:39">
+      <c r="C11" t="s">
+        <v>57</v>
+      </c>
+      <c r="D11" t="s">
+        <v>58</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="Q11">
+        <v>1</v>
+      </c>
+      <c r="S11">
+        <v>1</v>
+      </c>
+      <c r="AB11">
+        <v>1</v>
+      </c>
+      <c r="AC11">
+        <v>1</v>
+      </c>
+      <c r="AD11">
+        <v>1</v>
+      </c>
+      <c r="AG11">
+        <v>1</v>
+      </c>
+      <c r="AI11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:39">
+      <c r="C12" t="s">
+        <v>59</v>
+      </c>
+      <c r="D12" t="s">
+        <v>60</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="Q12">
+        <v>1</v>
+      </c>
+      <c r="R12">
+        <v>1</v>
+      </c>
+      <c r="S12">
+        <v>1</v>
+      </c>
+      <c r="AB12">
+        <v>1</v>
+      </c>
+      <c r="AC12">
+        <v>1</v>
+      </c>
+      <c r="AD12">
+        <v>1</v>
+      </c>
+      <c r="AI12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:39">
+      <c r="C13" t="s">
+        <v>61</v>
+      </c>
+      <c r="D13" t="s">
+        <v>62</v>
+      </c>
+      <c r="H13">
+        <v>1</v>
+      </c>
+      <c r="I13">
+        <v>1</v>
+      </c>
+      <c r="L13">
+        <v>1</v>
+      </c>
+      <c r="Q13">
+        <v>1</v>
+      </c>
+      <c r="AB13">
+        <v>1</v>
+      </c>
+      <c r="AC13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:39">
+      <c r="C14" t="s">
+        <v>63</v>
+      </c>
+      <c r="D14" t="s">
+        <v>64</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+      <c r="I14">
+        <v>1</v>
+      </c>
+      <c r="N14">
+        <v>1</v>
+      </c>
+      <c r="Q14">
+        <v>1</v>
+      </c>
+      <c r="AB14">
+        <v>1</v>
+      </c>
+      <c r="AC14">
+        <v>1</v>
+      </c>
+      <c r="AI14">
+        <v>1</v>
+      </c>
+      <c r="AK14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:39">
+      <c r="C15" t="s">
+        <v>65</v>
+      </c>
+      <c r="D15" t="s">
+        <v>66</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15">
+        <v>1</v>
+      </c>
+      <c r="I15">
+        <v>1</v>
+      </c>
+      <c r="K15">
+        <v>1</v>
+      </c>
+      <c r="L15">
+        <v>1</v>
+      </c>
+      <c r="Q15">
+        <v>1</v>
+      </c>
+      <c r="AB15">
+        <v>1</v>
+      </c>
+      <c r="AC15">
+        <v>1</v>
+      </c>
+      <c r="AD15">
+        <v>1</v>
+      </c>
+      <c r="AF15">
+        <v>1</v>
+      </c>
+      <c r="AI15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:39">
+      <c r="C16" t="s">
+        <v>67</v>
+      </c>
+      <c r="D16" t="s">
+        <v>68</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="H16">
+        <v>1</v>
+      </c>
+      <c r="I16">
+        <v>1</v>
+      </c>
+      <c r="L16">
+        <v>1</v>
+      </c>
+      <c r="Q16">
+        <v>1</v>
+      </c>
+      <c r="R16">
+        <v>1</v>
+      </c>
+      <c r="S16">
+        <v>1</v>
+      </c>
+      <c r="T16">
+        <v>1</v>
+      </c>
+      <c r="AB16">
+        <v>1</v>
+      </c>
+      <c r="AC16">
+        <v>1</v>
+      </c>
+      <c r="AI16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="3:37">
+      <c r="C17" t="s">
+        <v>69</v>
+      </c>
+      <c r="D17" t="s">
+        <v>70</v>
+      </c>
+      <c r="G17">
+        <v>1</v>
+      </c>
+      <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="I17">
+        <v>1</v>
+      </c>
+      <c r="Q17">
+        <v>1</v>
+      </c>
+      <c r="AB17">
+        <v>1</v>
+      </c>
+      <c r="AC17">
+        <v>1</v>
+      </c>
+      <c r="AI17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="3:37">
+      <c r="C18" t="s">
+        <v>71</v>
+      </c>
+      <c r="D18" t="s">
+        <v>72</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+      <c r="H18">
+        <v>1</v>
+      </c>
+      <c r="Q18">
+        <v>1</v>
+      </c>
+      <c r="S18">
+        <v>1</v>
+      </c>
+      <c r="AB18">
+        <v>1</v>
+      </c>
+      <c r="AC18">
+        <v>1</v>
+      </c>
+      <c r="AD18">
+        <v>1</v>
+      </c>
+      <c r="AI18">
+        <v>1</v>
+      </c>
+      <c r="AK18">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>